<commit_message>
odpowiedz na transmitancje policzona z intrukcji - matlab
</commit_message>
<xml_diff>
--- a/POMIARY.xlsx
+++ b/POMIARY.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t xml:space="preserve">1 zmierzyć czy filtr filtruje </t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Robimy to po to aby zpaisać to w postaci równania np.. U(t)=Ae^(-a*t)* cos(2*pi*f0*t)</t>
+  </si>
+  <si>
+    <t>Obliczone z instrukcji</t>
+  </si>
+  <si>
+    <t>f0 [Hz]</t>
   </si>
 </sst>
 </file>
@@ -778,11 +784,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="198275024"/>
-        <c:axId val="198277824"/>
+        <c:axId val="192219360"/>
+        <c:axId val="192219920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="198275024"/>
+        <c:axId val="192219360"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -835,7 +841,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -902,12 +907,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198277824"/>
+        <c:crossAx val="192219920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198277824"/>
+        <c:axId val="192219920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -958,7 +963,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1025,7 +1029,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198275024"/>
+        <c:crossAx val="192219360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1039,7 +1043,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1568,11 +1571,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="201410816"/>
-        <c:axId val="201411376"/>
+        <c:axId val="192222160"/>
+        <c:axId val="192222720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="201410816"/>
+        <c:axId val="192222160"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1625,7 +1628,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1692,12 +1694,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201411376"/>
+        <c:crossAx val="192222720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="201411376"/>
+        <c:axId val="192222720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1752,7 +1754,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1819,7 +1820,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201410816"/>
+        <c:crossAx val="192222160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1833,7 +1834,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3366,13 +3366,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="32.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3458,6 +3458,9 @@
       <c r="A16" t="s">
         <v>18</v>
       </c>
+      <c r="H16" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H17">
@@ -3512,10 +3515,6 @@
       <c r="B22">
         <v>320</v>
       </c>
-      <c r="H22">
-        <f>H21/2</f>
-        <v>1.36</v>
-      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -3528,7 +3527,7 @@
         <v>31</v>
       </c>
       <c r="H23" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I23" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
w sumie to nic
</commit_message>
<xml_diff>
--- a/POMIARY.xlsx
+++ b/POMIARY.xlsx
@@ -3367,7 +3367,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3596,6 +3596,14 @@
         <f>B27+$B$26</f>
         <v>964</v>
       </c>
+      <c r="G27">
+        <f>(B26-B20)/3</f>
+        <v>258.66666666666669</v>
+      </c>
+      <c r="H27">
+        <f>1/G27*1000000</f>
+        <v>3865.9793814432987</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -3619,6 +3627,12 @@
       <c r="F29">
         <f t="shared" si="0"/>
         <v>1224</v>
+      </c>
+      <c r="I29">
+        <v>3.3971499999999999</v>
+      </c>
+      <c r="J29">
+        <v>2985.53</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>